<commit_message>
Schema completed, todo: validate data using schema, then fix
</commit_message>
<xml_diff>
--- a/docs/cur_data_vs_cur_schema.xlsx
+++ b/docs/cur_data_vs_cur_schema.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/satria/google/PROMOVENDUS/mibig2/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/satria/google/PROMOVENDUS/mibig_schema_refactoring/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="14260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="properties_not_exist_in_schema" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="191">
   <si>
     <t>property</t>
   </si>
@@ -109,9 +109,6 @@
     <t>/general_params/genes/gene[]/gene_pubs[]</t>
   </si>
   <si>
-    <t>/general_params/Polyketide/Saccharide</t>
-  </si>
-  <si>
     <t>/general_params/Polyketide/Saccharide/gt_genes[]</t>
   </si>
   <si>
@@ -121,76 +118,40 @@
     <t>comments</t>
   </si>
   <si>
-    <t>/general_params</t>
-  </si>
-  <si>
-    <t>/general_params/Alkaloid</t>
-  </si>
-  <si>
-    <t>/general_params/NRP</t>
-  </si>
-  <si>
     <t>/general_params/NRP/nrps_genes[]</t>
   </si>
   <si>
     <t>/general_params/NRP/nrps_genes[]/nrps_module[]</t>
   </si>
   <si>
-    <t>/general_params/NRP/nrps_genes[]/nrps_module[]/a_substr_spec</t>
-  </si>
-  <si>
-    <t>/general_params/Other</t>
-  </si>
-  <si>
-    <t>/general_params/Polyketide</t>
-  </si>
-  <si>
     <t>/general_params/Polyketide/mod_pks_genes[]</t>
   </si>
   <si>
     <t>/general_params/Polyketide/mod_pks_genes[]/pks_module[]</t>
   </si>
   <si>
-    <t>/general_params/RiPP</t>
-  </si>
-  <si>
     <t>/general_params/RiPP/precursor_loci[]</t>
   </si>
   <si>
     <t>/general_params/RiPP/precursor_loci[]/crosslinks[]</t>
   </si>
   <si>
-    <t>/general_params/Saccharide</t>
-  </si>
-  <si>
     <t>/general_params/Saccharide/gt_genes[]</t>
   </si>
   <si>
-    <t>/general_params/Terpene</t>
-  </si>
-  <si>
     <t>/general_params/compounds[]</t>
   </si>
   <si>
     <t>/general_params/compounds[]/chem_moieties[]</t>
   </si>
   <si>
-    <t>/general_params/genes</t>
-  </si>
-  <si>
     <t>/general_params/genes/gene[]</t>
   </si>
   <si>
     <t>/general_params/genes/operon[]</t>
   </si>
   <si>
-    <t>/general_params/loci</t>
-  </si>
-  <si>
     <t>/general_params/loci/nucl_acc[]</t>
-  </si>
-  <si>
-    <t>/personal</t>
   </si>
   <si>
     <t>required</t>
@@ -735,21 +696,7 @@
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1030,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1049,27 +996,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1080,10 +1027,10 @@
         <v>1816</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1094,10 +1041,10 @@
         <v>494</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1108,24 +1055,24 @@
         <v>161</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1136,10 +1083,10 @@
         <v>494</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1150,10 +1097,10 @@
         <v>834</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1164,10 +1111,10 @@
         <v>92</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1178,80 +1125,80 @@
         <v>399</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1262,10 +1209,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1276,10 +1223,10 @@
         <v>86</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1290,24 +1237,24 @@
         <v>493</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B19">
         <v>1322</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1318,24 +1265,24 @@
         <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B21">
         <v>7</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1346,10 +1293,10 @@
         <v>163</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1360,24 +1307,24 @@
         <v>154</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1388,10 +1335,10 @@
         <v>168</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1402,10 +1349,10 @@
         <v>115</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1416,10 +1363,10 @@
         <v>120</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1430,10 +1377,10 @@
         <v>711</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1444,10 +1391,10 @@
         <v>60</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1458,164 +1405,150 @@
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B35">
-        <v>28</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>64</v>
+        <v>1192</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B36">
-        <v>1192</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B37">
         <v>69</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="B38">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D39" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B40">
         <v>22</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41">
-        <v>22</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1624,8 +1557,8 @@
       <sortCondition ref="A1:A36"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A2:D41">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A2:D40">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$C2="schema"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1635,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B146"/>
+  <dimension ref="A1:B133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A149" sqref="A149"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1652,17 +1585,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
       <c r="B2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -1670,23 +1606,23 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -1694,7 +1630,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1702,7 +1638,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -1710,7 +1646,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -1718,7 +1654,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
@@ -1726,7 +1662,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>
@@ -1734,15 +1670,15 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
@@ -1750,7 +1686,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
@@ -1758,15 +1694,15 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B16" t="b">
         <v>0</v>
@@ -1774,7 +1710,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -1782,23 +1718,23 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -1806,31 +1742,31 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -1838,7 +1774,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -1846,55 +1782,55 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -1902,15 +1838,15 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="B33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -1918,7 +1854,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
@@ -1926,15 +1862,15 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>31</v>
       </c>
       <c r="B36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B37" t="b">
         <v>0</v>
@@ -1942,7 +1878,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -1950,63 +1886,63 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="B41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
       <c r="B43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B46" t="b">
         <v>0</v>
@@ -2014,15 +1950,15 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B48" t="b">
         <v>1</v>
@@ -2030,15 +1966,15 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B50" t="b">
         <v>1</v>
@@ -2046,7 +1982,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B51" t="b">
         <v>1</v>
@@ -2054,15 +1990,15 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B53" t="b">
         <v>0</v>
@@ -2070,7 +2006,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B54" t="b">
         <v>1</v>
@@ -2078,7 +2014,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B55" t="b">
         <v>1</v>
@@ -2086,7 +2022,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B56" t="b">
         <v>0</v>
@@ -2094,7 +2030,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B57" t="b">
         <v>1</v>
@@ -2102,7 +2038,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="B58" t="b">
         <v>1</v>
@@ -2110,15 +2046,15 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B60" t="b">
         <v>0</v>
@@ -2126,23 +2062,23 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>130</v>
+        <v>33</v>
       </c>
       <c r="B61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B63" t="b">
         <v>0</v>
@@ -2150,31 +2086,31 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>39</v>
+        <v>125</v>
       </c>
       <c r="B64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="B66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B67" t="b">
         <v>0</v>
@@ -2182,7 +2118,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B68" t="b">
         <v>0</v>
@@ -2190,7 +2126,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="B69" t="b">
         <v>0</v>
@@ -2198,15 +2134,15 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>34</v>
       </c>
       <c r="B71" t="b">
         <v>0</v>
@@ -2214,23 +2150,23 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B74" t="b">
         <v>1</v>
@@ -2238,7 +2174,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B75" t="b">
         <v>0</v>
@@ -2246,7 +2182,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B76" t="b">
         <v>0</v>
@@ -2254,55 +2190,55 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="B79" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="B80" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B81" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B83" t="b">
         <v>1</v>
@@ -2310,23 +2246,23 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>148</v>
+        <v>35</v>
       </c>
       <c r="B84" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B86" t="b">
         <v>1</v>
@@ -2334,7 +2270,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B87" t="b">
         <v>0</v>
@@ -2342,7 +2278,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B88" t="b">
         <v>0</v>
@@ -2350,31 +2286,31 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B89" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B91" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B92" t="b">
         <v>0</v>
@@ -2382,23 +2318,23 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B93" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>45</v>
+        <v>152</v>
       </c>
       <c r="B94" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B95" t="b">
         <v>1</v>
@@ -2406,7 +2342,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B96" t="b">
         <v>1</v>
@@ -2414,7 +2350,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>46</v>
+        <v>155</v>
       </c>
       <c r="B97" t="b">
         <v>0</v>
@@ -2422,15 +2358,15 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B98" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B99" t="b">
         <v>0</v>
@@ -2438,7 +2374,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B100" t="b">
         <v>0</v>
@@ -2446,7 +2382,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B101" t="b">
         <v>0</v>
@@ -2454,7 +2390,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B102" t="b">
         <v>0</v>
@@ -2462,7 +2398,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B103" t="b">
         <v>0</v>
@@ -2470,7 +2406,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B104" t="b">
         <v>1</v>
@@ -2478,15 +2414,15 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
       <c r="B105" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B106" t="b">
         <v>1</v>
@@ -2494,7 +2430,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B107" t="b">
         <v>0</v>
@@ -2502,39 +2438,39 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B108" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B109" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B110" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B111" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B112" t="b">
         <v>0</v>
@@ -2542,7 +2478,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B113" t="b">
         <v>0</v>
@@ -2550,7 +2486,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B114" t="b">
         <v>1</v>
@@ -2558,7 +2494,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>47</v>
+        <v>172</v>
       </c>
       <c r="B115" t="b">
         <v>0</v>
@@ -2566,7 +2502,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>48</v>
+        <v>173</v>
       </c>
       <c r="B116" t="b">
         <v>0</v>
@@ -2574,7 +2510,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B117" t="b">
         <v>1</v>
@@ -2582,7 +2518,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>177</v>
+        <v>38</v>
       </c>
       <c r="B118" t="b">
         <v>0</v>
@@ -2590,7 +2526,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B119" t="b">
         <v>0</v>
@@ -2598,15 +2534,15 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B120" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B121" t="b">
         <v>1</v>
@@ -2614,7 +2550,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>181</v>
+        <v>39</v>
       </c>
       <c r="B122" t="b">
         <v>1</v>
@@ -2622,31 +2558,31 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B123" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B124" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B125" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B126" t="b">
         <v>0</v>
@@ -2654,7 +2590,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B127" t="b">
         <v>0</v>
@@ -2662,7 +2598,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B128" t="b">
         <v>1</v>
@@ -2670,7 +2606,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>49</v>
+        <v>184</v>
       </c>
       <c r="B129" t="b">
         <v>0</v>
@@ -2678,137 +2614,33 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B130" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B131" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>50</v>
+        <v>187</v>
       </c>
       <c r="B132" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B133" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>51</v>
-      </c>
-      <c r="B134" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>191</v>
-      </c>
-      <c r="B135" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>192</v>
-      </c>
-      <c r="B136" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>193</v>
-      </c>
-      <c r="B137" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>194</v>
-      </c>
-      <c r="B138" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>195</v>
-      </c>
-      <c r="B139" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>196</v>
-      </c>
-      <c r="B140" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>197</v>
-      </c>
-      <c r="B141" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>52</v>
-      </c>
-      <c r="B142" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>198</v>
-      </c>
-      <c r="B143" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>199</v>
-      </c>
-      <c r="B144" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>200</v>
-      </c>
-      <c r="B145" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
-        <v>201</v>
-      </c>
-      <c r="B146" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>